<commit_message>
20.04.2017 tarihli Veritabanı örnekleri
</commit_message>
<xml_diff>
--- a/Veritabani/Öğrenciler.xlsx
+++ b/Veritabani/Öğrenciler.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pau\Documents\Visual Studio 2012\Projects\nyp_ybs\Veritabanı\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pau\Documents\Visual Studio 2012\Projects\nyp_ybs\Veritabani\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
   <si>
     <t>Öğr.No.</t>
   </si>
@@ -44,55 +44,52 @@
     <t>Cinsiyet</t>
   </si>
   <si>
-    <t>Ömer</t>
-  </si>
-  <si>
-    <t>Mermer</t>
-  </si>
-  <si>
     <t>YBS</t>
   </si>
   <si>
     <t>E</t>
   </si>
   <si>
-    <t>Mine</t>
-  </si>
-  <si>
-    <t>Gülcü</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
-    <t>Durukan</t>
-  </si>
-  <si>
-    <t>Küpeli</t>
-  </si>
-  <si>
-    <t>Oğuzhan</t>
-  </si>
-  <si>
-    <t>Zor</t>
-  </si>
-  <si>
-    <t>Burak</t>
-  </si>
-  <si>
-    <t>Atalay</t>
-  </si>
-  <si>
-    <t>Şelale</t>
-  </si>
-  <si>
-    <t>Ersevinç</t>
-  </si>
-  <si>
-    <t>Elif</t>
-  </si>
-  <si>
-    <t>Erdem</t>
+    <t>Ali Eren</t>
+  </si>
+  <si>
+    <t>Sugeçmez</t>
+  </si>
+  <si>
+    <t>Merve</t>
+  </si>
+  <si>
+    <t>Gültekin</t>
+  </si>
+  <si>
+    <t>Sultan</t>
+  </si>
+  <si>
+    <t>Erdoğan</t>
+  </si>
+  <si>
+    <t>Mustafa</t>
+  </si>
+  <si>
+    <t>Özgün</t>
+  </si>
+  <si>
+    <t>Tansu</t>
+  </si>
+  <si>
+    <t>Gökçe</t>
+  </si>
+  <si>
+    <t>Mehmet</t>
+  </si>
+  <si>
+    <t>Eskicioğlu</t>
+  </si>
+  <si>
+    <t>S.No.</t>
   </si>
 </sst>
 </file>
@@ -159,11 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -444,19 +440,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,161 +480,138 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>14219503</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="B2">
+        <v>14219022</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2">
+        <v>35102</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="G2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="3">
-        <v>31294</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
-        <v>15219019</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="B3">
+        <v>15219020</v>
+      </c>
+      <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3">
-        <v>35218</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2">
+        <v>34965</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" t="s">
         <v>8</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="2">
-        <v>15219029</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B4">
+        <v>16219014</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3">
-        <v>35287</v>
-      </c>
-      <c r="F4" s="2" t="s">
+      <c r="E4" s="2">
+        <v>35453</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
         <v>8</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="2">
-        <v>16220503</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="B5">
+        <v>15219505</v>
+      </c>
+      <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="3">
-        <v>35403</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>9</v>
+      <c r="E5" s="2">
+        <v>34750</v>
+      </c>
+      <c r="F5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2">
-        <v>14219504</v>
-      </c>
-      <c r="C6" s="2" t="s">
+      <c r="B6">
+        <v>15219018</v>
+      </c>
+      <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3">
-        <v>34387</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="E6" s="2">
+        <v>35665</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
         <v>8</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>15219017</v>
-      </c>
-      <c r="C7" s="2" t="s">
+      <c r="B7">
+        <v>14219007</v>
+      </c>
+      <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="3">
-        <v>35251</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="E7" s="2">
+        <v>35065</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" t="s">
         <v>7</v>
-      </c>
-      <c r="B8" s="2">
-        <v>14219006</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="3">
-        <v>35065</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>